<commit_message>
adding alert and debug the error
</commit_message>
<xml_diff>
--- a/kotoba.xlsx
+++ b/kotoba.xlsx
@@ -2584,7 +2584,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2895,9 +2895,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2914,6 +2911,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3213,7 +3213,7 @@
   <dimension ref="A1:AE15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="26.25" customHeight="1"/>
@@ -3278,13 +3278,13 @@
       <c r="Z1" s="10">
         <v>11</v>
       </c>
-      <c r="AA1" s="30">
+      <c r="AA1" s="29">
         <v>12</v>
       </c>
-      <c r="AB1" s="28">
+      <c r="AB1" s="10">
         <v>13</v>
       </c>
-      <c r="AC1" s="33">
+      <c r="AC1" s="32">
         <v>14</v>
       </c>
       <c r="AD1" s="2"/>
@@ -3326,7 +3326,7 @@
       <c r="T2" s="11">
         <v>19</v>
       </c>
-      <c r="U2" s="31">
+      <c r="U2" s="34">
         <v>20</v>
       </c>
       <c r="V2" s="27">
@@ -3475,7 +3475,7 @@
       <c r="Y4" s="11">
         <v>52</v>
       </c>
-      <c r="Z4" s="31">
+      <c r="Z4" s="30">
         <v>53</v>
       </c>
       <c r="AA4" s="27">
@@ -3484,7 +3484,7 @@
       <c r="AB4" s="27">
         <v>55</v>
       </c>
-      <c r="AC4" s="34">
+      <c r="AC4" s="33">
         <v>56</v>
       </c>
       <c r="AD4" s="2"/>
@@ -3603,10 +3603,10 @@
         <v>12</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="32">
+      <c r="P6" s="31">
         <v>71</v>
       </c>
-      <c r="Q6" s="27">
+      <c r="Q6" s="34">
         <v>72</v>
       </c>
       <c r="R6" s="27">
@@ -3618,7 +3618,7 @@
       <c r="T6" s="27">
         <v>75</v>
       </c>
-      <c r="U6" s="27">
+      <c r="U6" s="34">
         <v>76</v>
       </c>
       <c r="V6" s="27">
@@ -3630,7 +3630,7 @@
       <c r="X6" s="27">
         <v>79</v>
       </c>
-      <c r="Y6" s="27">
+      <c r="Y6" s="34">
         <v>80</v>
       </c>
       <c r="Z6" s="27">
@@ -3642,7 +3642,7 @@
       <c r="AB6" s="27">
         <v>83</v>
       </c>
-      <c r="AC6" s="34">
+      <c r="AC6" s="33">
         <v>84</v>
       </c>
       <c r="AD6" s="2"/>
@@ -3824,7 +3824,7 @@
       <c r="X9" s="11">
         <v>121</v>
       </c>
-      <c r="Y9" s="31">
+      <c r="Y9" s="34">
         <v>122</v>
       </c>
       <c r="Z9" s="27">
@@ -3895,7 +3895,7 @@
       <c r="Y10" s="11">
         <v>136</v>
       </c>
-      <c r="Z10" s="27">
+      <c r="Z10" s="34">
         <v>137</v>
       </c>
       <c r="AA10" s="27">
@@ -3952,10 +3952,10 @@
       <c r="T11" s="11">
         <v>145</v>
       </c>
-      <c r="U11" s="31">
+      <c r="U11" s="30">
         <v>146</v>
       </c>
-      <c r="V11" s="27">
+      <c r="V11" s="34">
         <v>147</v>
       </c>
       <c r="W11" s="27">
@@ -4082,10 +4082,10 @@
       <c r="T13" s="11">
         <v>173</v>
       </c>
-      <c r="U13" s="31">
+      <c r="U13" s="30">
         <v>174</v>
       </c>
-      <c r="V13" s="27">
+      <c r="V13" s="34">
         <v>175</v>
       </c>
       <c r="W13" s="27">
@@ -4147,7 +4147,7 @@
       <c r="U14" s="14">
         <v>188</v>
       </c>
-      <c r="V14" s="29">
+      <c r="V14" s="28">
         <v>189</v>
       </c>
       <c r="W14" s="14">

</xml_diff>